<commit_message>
Incorporated ds2 into SGR vs. MR modeling and fixes to models that require an individual level random effect.
</commit_message>
<xml_diff>
--- a/001_Raw_Data/DS3_Skeeles2024.xlsx
+++ b/001_Raw_Data/DS3_Skeeles2024.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{DCABF3F3-E053-4112-9E2E-71669D9428C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44268980-9059-4549-BA0F-5B30A2D182E8}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{DCABF3F3-E053-4112-9E2E-71669D9428C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6887145-1641-463B-A507-9B63990CE153}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Beth Sheet" sheetId="4" r:id="rId1"/>
@@ -1528,6 +1528,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1535,7 +1536,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -8882,12 +8882,13 @@
   <dimension ref="A1:AE29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="67" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.35">

</xml_diff>